<commit_message>
Ajustes no extrato de comissão
</commit_message>
<xml_diff>
--- a/Workflow/Workflow/Presentation.Web/wwwroot/templates/TEMPLATE_EXTRATO_COMISSAO.xlsx
+++ b/Workflow/Workflow/Presentation.Web/wwwroot/templates/TEMPLATE_EXTRATO_COMISSAO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ledim\source\repos\BMG Seguros\Workflow\Workflow\Presentation.Web\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150C8775-57B8-40C3-9C0B-D23EC2DE396E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D14FD9-1C98-4E96-9169-3C08A2EA2917}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,12 +274,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -287,6 +281,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,7 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="0"/>
     <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -453,122 +453,77 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -604,27 +559,6 @@
     <xf numFmtId="14" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="13" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -637,12 +571,7 @@
     <xf numFmtId="1" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -658,6 +587,65 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -995,32 +983,32 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="28">
         <v>1</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="43"/>
-      <c r="S2" s="44"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="37"/>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
@@ -1102,28 +1090,28 @@
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
       <c r="O6" s="20"/>
-      <c r="P6" s="45" t="s">
+      <c r="P6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="47"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="40"/>
     </row>
     <row r="7" spans="2:19" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="73"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="91"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="93"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="66"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -1131,140 +1119,140 @@
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="76"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="75"/>
     </row>
     <row r="10" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="86"/>
+      <c r="D10" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29" t="s">
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="29" t="s">
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="27" t="s">
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="28"/>
+      <c r="Q10" s="87"/>
+      <c r="R10" s="87"/>
+      <c r="S10" s="86"/>
     </row>
     <row r="11" spans="2:19" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="89"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="87"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="85"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="87"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="78"/>
+      <c r="P11" s="76"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="77"/>
+      <c r="S11" s="78"/>
     </row>
     <row r="12" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="75"/>
-      <c r="N13" s="75"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="75"/>
-      <c r="S13" s="76"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="75"/>
     </row>
     <row r="14" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="24" t="s">
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="24" t="s">
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="25"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="90"/>
     </row>
     <row r="15" spans="2:19" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="71"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="72"/>
+      <c r="G15" s="57"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="9"/>
-      <c r="N15" s="88"/>
+      <c r="N15" s="63"/>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
@@ -1275,52 +1263,52 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="76"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="75"/>
     </row>
     <row r="18" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="24" t="s">
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="24" t="s">
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="89"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="25"/>
+      <c r="O18" s="89"/>
+      <c r="P18" s="89"/>
+      <c r="Q18" s="89"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="90"/>
     </row>
     <row r="19" spans="2:19" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8"/>
@@ -1328,27 +1316,22 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
-      <c r="L19" s="85"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="86"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85"/>
-      <c r="R19" s="85"/>
-      <c r="S19" s="87"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="77"/>
+      <c r="M19" s="78"/>
+      <c r="N19" s="76"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="77"/>
+      <c r="Q19" s="77"/>
+      <c r="R19" s="77"/>
+      <c r="S19" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="B13:S13"/>
     <mergeCell ref="B17:S17"/>
     <mergeCell ref="B9:S9"/>
     <mergeCell ref="N19:S19"/>
@@ -1358,6 +1341,11 @@
     <mergeCell ref="H11:K11"/>
     <mergeCell ref="D11:G11"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="B13:S13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1368,9 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:S4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1381,52 +1367,52 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="76"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="75"/>
     </row>
     <row r="3" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="24" t="s">
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="25"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="90"/>
     </row>
     <row r="4" spans="2:19" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
@@ -1441,12 +1427,12 @@
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="87"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1462,9 +1448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:S4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1475,70 +1459,70 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="76"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="75"/>
     </row>
     <row r="3" spans="2:19" s="23" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="26" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="25"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="90"/>
     </row>
     <row r="4" spans="2:19" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="31"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="87"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1554,124 +1538,122 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:Z4"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="48" customWidth="1"/>
-    <col min="2" max="10" width="11.5703125" style="48" customWidth="1"/>
-    <col min="11" max="12" width="13" style="48" customWidth="1"/>
-    <col min="13" max="19" width="11.5703125" style="48" customWidth="1"/>
-    <col min="20" max="23" width="8.85546875" style="48"/>
-    <col min="24" max="24" width="9.42578125" style="48" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.85546875" style="48"/>
+    <col min="1" max="1" width="3" style="41" customWidth="1"/>
+    <col min="2" max="10" width="11.5703125" style="41" customWidth="1"/>
+    <col min="11" max="12" width="13" style="41" customWidth="1"/>
+    <col min="13" max="19" width="11.5703125" style="41" customWidth="1"/>
+    <col min="20" max="23" width="8.85546875" style="41"/>
+    <col min="24" max="24" width="9.42578125" style="41" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.85546875" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:26" s="52" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="79" t="s">
+    <row r="2" spans="2:26" s="45" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="80"/>
-      <c r="N2" s="80"/>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="51"/>
-    </row>
-    <row r="3" spans="2:26" s="61" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="53" t="s">
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="44"/>
+    </row>
+    <row r="3" spans="2:26" s="46" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="53" t="s">
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="53" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56" t="s">
+      <c r="I3" s="89"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="53" t="s">
+      <c r="M3" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="57" t="s">
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="90"/>
+      <c r="R3" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="57"/>
-      <c r="T3" s="53" t="s">
+      <c r="S3" s="87"/>
+      <c r="T3" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="55"/>
-      <c r="V3" s="53" t="s">
+      <c r="U3" s="90"/>
+      <c r="V3" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="59" t="s">
+      <c r="W3" s="93"/>
+      <c r="X3" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="Y3" s="60"/>
-      <c r="Z3" s="58"/>
-    </row>
-    <row r="4" spans="2:26" s="61" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="62"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="69"/>
-      <c r="W4" s="70"/>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="67"/>
-      <c r="Z4" s="68"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="93"/>
+    </row>
+    <row r="4" spans="2:26" s="46" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="55"/>
+      <c r="X4" s="51"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>